<commit_message>
finish dev of getLevelupReward
</commit_message>
<xml_diff>
--- a/gameData/shared/Activities.xlsx
+++ b/gameData/shared/Activities.xlsx
@@ -4,24 +4,29 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16140" yWindow="1000" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="1"/>
+    <workbookView xWindow="10740" yWindow="2720" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="day60" sheetId="24" r:id="rId1"/>
     <sheet name="online" sheetId="27" r:id="rId2"/>
     <sheet name="day14" sheetId="28" r:id="rId3"/>
+    <sheet name="levelup" sheetId="29" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="3">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8">#REF!</definedName>
   </definedNames>
@@ -35,61 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
-  <si>
-    <t>STR_itemName</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>movingConstruction</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>torch</t>
-  </si>
-  <si>
-    <t>changePlayerName</t>
-  </si>
-  <si>
-    <t>changeCityName</t>
-  </si>
-  <si>
-    <t>retreatTroop</t>
-  </si>
-  <si>
-    <t>moveTheCity</t>
-  </si>
-  <si>
-    <t>dragonExp_1</t>
-  </si>
-  <si>
-    <t>dragonExp_2</t>
-  </si>
-  <si>
-    <t>dragonExp_3</t>
-  </si>
-  <si>
-    <t>dragonHp_1</t>
-  </si>
-  <si>
-    <t>dragonHp_2</t>
-  </si>
-  <si>
-    <t>dragonHp_3</t>
-  </si>
-  <si>
-    <t>heroBlood_1</t>
-  </si>
-  <si>
-    <t>heroBlood_2</t>
-  </si>
-  <si>
-    <t>stamina_1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>stamina_2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="15">
   <si>
     <t>INT_day</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -114,15 +65,36 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>INT_itemCount</t>
+    <t>INT_onLineMinutes</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>STR_itemCount</t>
+    <t>INT_index</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>INT_onLineMinutes</t>
+    <t>INT_level</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_rewards</t>
+  </si>
+  <si>
+    <t>STR_rewards</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>special:movingConstruction:1,special:torch:1</t>
+  </si>
+  <si>
+    <t>special:movingConstruction:1,special:torch:1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>special:movingConstruction:1</t>
+  </si>
+  <si>
+    <t>special:movingConstruction:1</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -267,7 +239,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -282,6 +254,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -368,7 +356,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="96">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -411,6 +399,14 @@
     <cellStyle name="超链接" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -446,6 +442,14 @@
     <cellStyle name="访问过的超链接" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -895,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView showRuler="0" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -907,676 +911,493 @@
     <col min="2" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="20" customHeight="1">
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="20" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="20" customHeight="1">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="20" customHeight="1">
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="20" customHeight="1">
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="20" customHeight="1">
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="20" customHeight="1">
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="20" customHeight="1">
+    </row>
+    <row r="15" spans="1:4" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="20" customHeight="1">
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1">
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20" customHeight="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20" customHeight="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20" customHeight="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1">
+      <c r="B19" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20" customHeight="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20" customHeight="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1">
+      <c r="B21" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20" customHeight="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20" customHeight="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="20" customHeight="1">
+      <c r="B23" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20" customHeight="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20" customHeight="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="20" customHeight="1">
+      <c r="B25" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20" customHeight="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20" customHeight="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="20" customHeight="1">
+      <c r="B27" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20" customHeight="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20" customHeight="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="20" customHeight="1">
+      <c r="B29" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20" customHeight="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="20" customHeight="1">
+    </row>
+    <row r="31" spans="1:2" ht="20" customHeight="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="20" customHeight="1">
+      <c r="B31" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20" customHeight="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20" customHeight="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="20" customHeight="1">
+      <c r="B33" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="20" customHeight="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="20" customHeight="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="20" customHeight="1">
+      <c r="B35" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="20" customHeight="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="20" customHeight="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="20" customHeight="1">
+      <c r="B37" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="20" customHeight="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="20" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="20" customHeight="1">
+      <c r="B39" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="20" customHeight="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="20" customHeight="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="20" customHeight="1">
+      <c r="B41" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="20" customHeight="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="20" customHeight="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="20" customHeight="1">
+      <c r="B43" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="20" customHeight="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="20" customHeight="1">
+    </row>
+    <row r="45" spans="1:2" ht="20" customHeight="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="20" customHeight="1">
+      <c r="B45" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="20" customHeight="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="20" customHeight="1">
+      <c r="B46" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="20" customHeight="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="20" customHeight="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="20" customHeight="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="20" customHeight="1">
+      <c r="B49" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="20" customHeight="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="20" customHeight="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="20" customHeight="1">
+      <c r="B51" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="20" customHeight="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="20" customHeight="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="20" customHeight="1">
+      <c r="B53" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="20" customHeight="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="20" customHeight="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="20" customHeight="1">
+      <c r="B55" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="20" customHeight="1">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="20" customHeight="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="20" customHeight="1">
+      <c r="B57" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="20" customHeight="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="20" customHeight="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C59" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="20" customHeight="1">
+      <c r="B59" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="20" customHeight="1">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="20" customHeight="1">
+    </row>
+    <row r="61" spans="1:2" ht="20" customHeight="1">
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C61" s="1">
-        <v>1</v>
+      <c r="B61" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1593,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1605,22 +1426,19 @@
     <col min="2" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1628,27 +1446,21 @@
         <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>30</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1656,43 +1468,37 @@
         <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>120</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
@@ -1804,7 +1610,223 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="20.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="20" customHeight="1">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="2:2" ht="20" customHeight="1">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="20" spans="2:2" ht="20" customHeight="1">
+      <c r="B20" s="4"/>
+    </row>
+    <row r="22" spans="2:2" ht="20" customHeight="1">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="24" spans="2:2" ht="20" customHeight="1">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="26" spans="2:2" ht="20" customHeight="1">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="28" spans="2:2" ht="20" customHeight="1">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="30" spans="2:2" ht="20" customHeight="1">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="32" spans="2:2" ht="20" customHeight="1">
+      <c r="B32" s="4"/>
+    </row>
+    <row r="34" spans="2:2" ht="20" customHeight="1">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="36" spans="2:2" ht="20" customHeight="1">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="38" spans="2:2" ht="20" customHeight="1">
+      <c r="B38" s="4"/>
+    </row>
+    <row r="40" spans="2:2" ht="20" customHeight="1">
+      <c r="B40" s="4"/>
+    </row>
+    <row r="42" spans="2:2" ht="20" customHeight="1">
+      <c r="B42" s="4"/>
+    </row>
+    <row r="44" spans="2:2" ht="20" customHeight="1">
+      <c r="B44" s="4"/>
+    </row>
+    <row r="47" spans="2:2" ht="20" customHeight="1">
+      <c r="B47" s="4"/>
+    </row>
+    <row r="48" spans="2:2" ht="20" customHeight="1">
+      <c r="B48" s="4"/>
+    </row>
+    <row r="50" spans="2:2" ht="20" customHeight="1">
+      <c r="B50" s="4"/>
+    </row>
+    <row r="52" spans="2:2" ht="20" customHeight="1">
+      <c r="B52" s="4"/>
+    </row>
+    <row r="54" spans="2:2" ht="20" customHeight="1">
+      <c r="B54" s="4"/>
+    </row>
+    <row r="56" spans="2:2" ht="20" customHeight="1">
+      <c r="B56" s="4"/>
+    </row>
+    <row r="58" spans="2:2" ht="20" customHeight="1">
+      <c r="B58" s="4"/>
+    </row>
+    <row r="60" spans="2:2" ht="20" customHeight="1">
+      <c r="B60" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1816,10 +1838,13 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E1" s="3"/>
     </row>
@@ -1827,112 +1852,99 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
+      <c r="B4" s="1">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
+      <c r="B6" s="1">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
+      <c r="B7" s="1">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
+      <c r="B8" s="1">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
+      <c r="B9" s="1">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="20" customHeight="1">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="20" customHeight="1">
-      <c r="A12" s="1">
+      <c r="C10" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="20" customHeight="1">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="20" customHeight="1">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="20" customHeight="1">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="20" customHeight="1">

</xml_diff>